<commit_message>
ADDITION OF NUMBER OF PPRIZE
</commit_message>
<xml_diff>
--- a/extras/database.xlsx
+++ b/extras/database.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="75">
   <si>
     <t>NAME</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>USER_MESSAGE</t>
+  </si>
+  <si>
+    <t>TOURNAMENT_TOTAL_WINNER</t>
+  </si>
+  <si>
+    <t>COUNT OF TOTAL NUMBER OF PRIZE IN THAT EVENT</t>
   </si>
 </sst>
 </file>
@@ -461,17 +467,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -753,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H38"/>
+  <dimension ref="B1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D38" sqref="B34:D38"/>
+    <sheetView tabSelected="1" topLeftCell="C14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,196 +1094,207 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F22" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F23" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G23" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F23" s="12" t="s">
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F24" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G24" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H23" s="14"/>
-    </row>
-    <row r="24" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="2" t="s">
+      <c r="H24" s="14"/>
+    </row>
+    <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G26" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H26" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C27" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="F26" s="15" t="s">
+      <c r="D27" s="9"/>
+      <c r="F27" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G27" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="F27" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H27" s="7"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="7"/>
+      <c r="F28" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="F29" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G29" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="16" t="s">
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D30" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F30" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G30" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="16" t="s">
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="16" t="s">
         <v>47</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="18"/>
-      <c r="F30" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="H30" s="14"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="16" t="s">
-        <v>55</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D31" s="7"/>
-    </row>
-    <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="17" t="s">
+      <c r="D31" s="21"/>
+      <c r="F31" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H31" s="14"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C33" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="14"/>
-    </row>
-    <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="2" t="s">
+      <c r="D33" s="14"/>
+    </row>
+    <row r="34" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D35" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="19" t="s">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C36" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="9"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="20" t="s">
+      <c r="D36" s="9"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="19" t="s">
         <v>70</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="7"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="20" t="s">
-        <v>71</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D37" s="7"/>
     </row>
-    <row r="38" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="21" t="s">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="7"/>
+    </row>
+    <row r="39" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C39" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="14"/>
+      <c r="D39" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>